<commit_message>
Read from excel correctly
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcacevedo/TextBlasterRedux/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C99F33EF-ABE5-A746-8CE4-256E052BAFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D390D87-FDF9-7243-85E6-ECEB9CB95356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{5E4D3A03-8025-3640-9537-BC0896558AAE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>First Name</t>
   </si>
@@ -60,9 +60,6 @@
     <t>sss</t>
   </si>
   <si>
-    <t>123-123-1234</t>
-  </si>
-  <si>
     <t>Marc</t>
   </si>
   <si>
@@ -70,6 +67,12 @@
   </si>
   <si>
     <t>mcmacevedo</t>
+  </si>
+  <si>
+    <t>+17324061005</t>
+  </si>
+  <si>
+    <t>+11231231234</t>
   </si>
 </sst>
 </file>
@@ -105,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,63 +428,64 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
-        <v>17324061005</v>
-      </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>